<commit_message>
Auto-committed on 2022/05/25 週三 16:38:06.80
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L1-顧客管理作業/CustTelNo.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L1-顧客管理作業/CustTelNo.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L1-顧客管理作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B36757A-E291-423C-B752-3FC05A9D6AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
     <sheet name="DBS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -365,7 +366,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -608,8 +609,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="1"/>
-    <cellStyle name="一般 2 2" xfId="2"/>
+    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="一般 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -700,6 +701,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -735,6 +753,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -910,25 +945,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="21.453125" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.90625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="21.44140625" style="4"/>
+    <col min="7" max="7" width="27.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="21.453125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
         <v>23</v>
       </c>
@@ -943,7 +978,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="12" t="s">
@@ -956,7 +991,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="21" t="s">
         <v>25</v>
       </c>
@@ -969,7 +1004,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="21" t="s">
         <v>26</v>
       </c>
@@ -984,7 +1019,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="21" t="s">
         <v>27</v>
       </c>
@@ -997,7 +1032,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="21" t="s">
         <v>28</v>
       </c>
@@ -1008,7 +1043,7 @@
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="21" t="s">
         <v>29</v>
       </c>
@@ -1019,7 +1054,7 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="12" t="s">
         <v>30</v>
       </c>
@@ -1042,7 +1077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -1061,7 +1096,7 @@
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="18">
         <v>2</v>
       </c>
@@ -1080,7 +1115,7 @@
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="136" x14ac:dyDescent="0.4">
       <c r="A11" s="18">
         <v>3</v>
       </c>
@@ -1101,7 +1136,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="18">
         <v>4</v>
       </c>
@@ -1120,7 +1155,7 @@
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.4">
       <c r="A13" s="18">
         <v>5</v>
       </c>
@@ -1141,7 +1176,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="18">
         <v>6</v>
       </c>
@@ -1160,7 +1195,7 @@
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" ht="48.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.4">
       <c r="A15" s="18">
         <v>7</v>
       </c>
@@ -1181,7 +1216,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="243" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="255" x14ac:dyDescent="0.4">
       <c r="A16" s="18">
         <v>8</v>
       </c>
@@ -1202,7 +1237,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="18">
         <v>9</v>
       </c>
@@ -1221,7 +1256,7 @@
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="18">
         <v>10</v>
       </c>
@@ -1240,7 +1275,7 @@
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="18">
         <v>11</v>
       </c>
@@ -1259,7 +1294,7 @@
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
     </row>
-    <row r="20" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.4">
       <c r="A20" s="18">
         <v>12</v>
       </c>
@@ -1280,7 +1315,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="18">
         <v>13</v>
       </c>
@@ -1297,7 +1332,7 @@
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="18">
         <v>14</v>
       </c>
@@ -1316,7 +1351,7 @@
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="18">
         <v>15</v>
       </c>
@@ -1333,7 +1368,7 @@
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="18">
         <v>16</v>
       </c>
@@ -1352,7 +1387,7 @@
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -1361,7 +1396,7 @@
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -1370,7 +1405,7 @@
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -1379,7 +1414,7 @@
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="18"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
@@ -1388,7 +1423,7 @@
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
@@ -1397,7 +1432,7 @@
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
@@ -1406,7 +1441,7 @@
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -1415,7 +1450,7 @@
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" s="18"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -1424,7 +1459,7 @@
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" s="18"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -1433,7 +1468,7 @@
       <c r="F33" s="18"/>
       <c r="G33" s="18"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" s="18"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -1442,7 +1477,7 @@
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" s="18"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -1451,7 +1486,7 @@
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -1460,7 +1495,7 @@
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -1469,7 +1504,7 @@
       <c r="F37" s="18"/>
       <c r="G37" s="18"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38" s="18"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -1478,7 +1513,7 @@
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -1487,7 +1522,7 @@
       <c r="F39" s="18"/>
       <c r="G39" s="18"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
@@ -1496,7 +1531,7 @@
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
@@ -1505,7 +1540,7 @@
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" s="18"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -1514,7 +1549,7 @@
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" s="18"/>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
@@ -1523,7 +1558,7 @@
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
       <c r="C44" s="18"/>
@@ -1532,7 +1567,7 @@
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
@@ -1541,7 +1576,7 @@
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -1550,7 +1585,7 @@
       <c r="F46" s="18"/>
       <c r="G46" s="18"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" s="18"/>
       <c r="B47" s="18"/>
       <c r="C47" s="18"/>
@@ -1559,7 +1594,7 @@
       <c r="F47" s="18"/>
       <c r="G47" s="18"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" s="18"/>
       <c r="B48" s="18"/>
       <c r="C48" s="18"/>
@@ -1568,7 +1603,7 @@
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
       <c r="C49" s="18"/>
@@ -1577,7 +1612,7 @@
       <c r="F49" s="18"/>
       <c r="G49" s="18"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
@@ -1586,7 +1621,7 @@
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51" s="18"/>
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
@@ -1595,7 +1630,7 @@
       <c r="F51" s="18"/>
       <c r="G51" s="18"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52" s="18"/>
       <c r="B52" s="18"/>
       <c r="C52" s="18"/>
@@ -1604,7 +1639,7 @@
       <c r="F52" s="18"/>
       <c r="G52" s="18"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A53" s="18"/>
       <c r="B53" s="18"/>
       <c r="C53" s="18"/>
@@ -1613,7 +1648,7 @@
       <c r="F53" s="18"/>
       <c r="G53" s="18"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54" s="18"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
@@ -1622,7 +1657,7 @@
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A55" s="18"/>
       <c r="B55" s="18"/>
       <c r="C55" s="18"/>
@@ -1631,7 +1666,7 @@
       <c r="F55" s="18"/>
       <c r="G55" s="18"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A56" s="18"/>
       <c r="B56" s="18"/>
       <c r="C56" s="18"/>
@@ -1640,7 +1675,7 @@
       <c r="F56" s="18"/>
       <c r="G56" s="18"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A57" s="18"/>
       <c r="B57" s="18"/>
       <c r="C57" s="18"/>
@@ -1649,7 +1684,7 @@
       <c r="F57" s="18"/>
       <c r="G57" s="18"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A58" s="18"/>
       <c r="B58" s="18"/>
       <c r="C58" s="18"/>
@@ -1658,7 +1693,7 @@
       <c r="F58" s="18"/>
       <c r="G58" s="18"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A59" s="18"/>
       <c r="B59" s="18"/>
       <c r="C59" s="18"/>
@@ -1667,7 +1702,7 @@
       <c r="F59" s="18"/>
       <c r="G59" s="18"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A60" s="18"/>
       <c r="B60" s="18"/>
       <c r="C60" s="18"/>
@@ -1676,7 +1711,7 @@
       <c r="F60" s="18"/>
       <c r="G60" s="18"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A61" s="18"/>
       <c r="B61" s="18"/>
       <c r="C61" s="18"/>
@@ -1685,7 +1720,7 @@
       <c r="F61" s="18"/>
       <c r="G61" s="18"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A62" s="18"/>
       <c r="B62" s="18"/>
       <c r="C62" s="18"/>
@@ -1694,7 +1729,7 @@
       <c r="F62" s="18"/>
       <c r="G62" s="18"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A63" s="18"/>
       <c r="B63" s="18"/>
       <c r="C63" s="18"/>
@@ -1703,7 +1738,7 @@
       <c r="F63" s="18"/>
       <c r="G63" s="18"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A64" s="18"/>
       <c r="B64" s="18"/>
       <c r="C64" s="18"/>
@@ -1712,7 +1747,7 @@
       <c r="F64" s="18"/>
       <c r="G64" s="18"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A65" s="18"/>
       <c r="B65" s="18"/>
       <c r="C65" s="18"/>
@@ -1721,7 +1756,7 @@
       <c r="F65" s="18"/>
       <c r="G65" s="18"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A66" s="18"/>
       <c r="B66" s="18"/>
       <c r="C66" s="18"/>
@@ -1730,7 +1765,7 @@
       <c r="F66" s="18"/>
       <c r="G66" s="18"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A67" s="18"/>
       <c r="B67" s="18"/>
       <c r="C67" s="18"/>
@@ -1739,7 +1774,7 @@
       <c r="F67" s="18"/>
       <c r="G67" s="18"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A68" s="18"/>
       <c r="B68" s="18"/>
       <c r="C68" s="18"/>
@@ -1748,7 +1783,7 @@
       <c r="F68" s="18"/>
       <c r="G68" s="18"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A69" s="18"/>
       <c r="B69" s="18"/>
       <c r="C69" s="18"/>
@@ -1757,7 +1792,7 @@
       <c r="F69" s="18"/>
       <c r="G69" s="18"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A70" s="18"/>
       <c r="B70" s="18"/>
       <c r="C70" s="18"/>
@@ -1766,7 +1801,7 @@
       <c r="F70" s="18"/>
       <c r="G70" s="18"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A71" s="18"/>
       <c r="B71" s="18"/>
       <c r="C71" s="18"/>
@@ -1792,23 +1827,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.08984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.6328125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1819,7 +1854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -1830,7 +1865,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -1841,7 +1876,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="20" t="s">
         <v>63</v>
       </c>

</xml_diff>